<commit_message>
updated my reads post draft, index, and academic blog front pages
</commit_message>
<xml_diff>
--- a/data/my-reads.xlsx
+++ b/data/my-reads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Desktop/github-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685833C3-EFFD-8141-940F-948D2C2DBF0E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454CF0DA-44F5-0341-95E8-1461948A6F72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{6A43893A-E979-8943-8C08-0CBFF629ACEC}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="reading-data" sheetId="1" r:id="rId1"/>
     <sheet name="book-list" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:G367"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,6 +521,12 @@
         <f>WEEKNUM(A4)</f>
         <v>1</v>
       </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -540,6 +546,12 @@
       </c>
       <c r="E5">
         <f>WEEKNUM(A5)</f>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated my reads data
</commit_message>
<xml_diff>
--- a/data/my-reads.xlsx
+++ b/data/my-reads.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Library/Mobile Documents/com~apple~CloudDocs/Desktop/github-website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Desktop/github-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4C2EDD-796A-8B4A-941D-8C0B8AF0F241}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1665D229-13C8-C247-9203-D216451B9DCF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="800" windowWidth="25440" windowHeight="15000" activeTab="1" xr2:uid="{6A43893A-E979-8943-8C08-0CBFF629ACEC}"/>
+    <workbookView xWindow="160" yWindow="800" windowWidth="25440" windowHeight="15000" activeTab="1" xr2:uid="{6A43893A-E979-8943-8C08-0CBFF629ACEC}"/>
   </bookViews>
   <sheets>
     <sheet name="reading-data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>date</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>An Introduction to the Event-Related Potential Technique (2nd e.)</t>
+  </si>
+  <si>
+    <t>book.year</t>
   </si>
 </sst>
 </file>
@@ -8230,13 +8233,13 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8248,7 +8251,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
update my reads data
</commit_message>
<xml_diff>
--- a/data/my-reads.xlsx
+++ b/data/my-reads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Desktop/github-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1665D229-13C8-C247-9203-D216451B9DCF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D859485D-814D-B14B-8FCB-03E3F33713CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="800" windowWidth="25440" windowHeight="15000" activeTab="1" xr2:uid="{6A43893A-E979-8943-8C08-0CBFF629ACEC}"/>
+    <workbookView xWindow="160" yWindow="800" windowWidth="25440" windowHeight="15000" xr2:uid="{6A43893A-E979-8943-8C08-0CBFF629ACEC}"/>
   </bookViews>
   <sheets>
     <sheet name="reading-data" sheetId="1" r:id="rId1"/>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F081B7-288B-1045-AB76-1CD03FBCB65E}">
   <dimension ref="A1:G368"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,6 +746,12 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
+      <c r="F12">
+        <v>18</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -767,6 +773,12 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -788,6 +800,12 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -809,6 +827,12 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
+      <c r="F15">
+        <v>20</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -829,6 +853,12 @@
       <c r="E16">
         <f t="shared" si="3"/>
         <v>3</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -8232,7 +8262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082B48B6-1501-774C-818C-F75B39B01AEE}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
final draft of nhl pca post
</commit_message>
<xml_diff>
--- a/data/my-reads.xlsx
+++ b/data/my-reads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Library/Mobile Documents/com~apple~CloudDocs/Desktop/github-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B8ADD3-C516-904C-836C-C76C1121C480}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700E1065-C59F-204F-B94B-4E553185B10E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="1540" windowWidth="25440" windowHeight="15000" xr2:uid="{6A43893A-E979-8943-8C08-0CBFF629ACEC}"/>
+    <workbookView xWindow="3200" yWindow="1780" windowWidth="25440" windowHeight="15000" xr2:uid="{6A43893A-E979-8943-8C08-0CBFF629ACEC}"/>
   </bookViews>
   <sheets>
     <sheet name="reading-data" sheetId="1" r:id="rId1"/>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F081B7-288B-1045-AB76-1CD03FBCB65E}">
   <dimension ref="A1:G369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1536,7 +1536,7 @@
         <v>6</v>
       </c>
       <c r="F41">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G41">
         <v>3</v>
@@ -1562,6 +1562,12 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
+      <c r="F42">
+        <v>19</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -1583,6 +1589,12 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
+      <c r="F43">
+        <v>15</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -1604,6 +1616,12 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
+      <c r="F44">
+        <v>17</v>
+      </c>
+      <c r="G44">
+        <v>3</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -1625,6 +1643,12 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -1646,6 +1670,12 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
+      <c r="F46">
+        <v>22</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -1667,6 +1697,12 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>3</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -1688,8 +1724,14 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>7</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43510</v>
       </c>
@@ -1709,8 +1751,14 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>13</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43511</v>
       </c>
@@ -1730,8 +1778,14 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>19</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43512</v>
       </c>
@@ -1751,8 +1805,14 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>11</v>
+      </c>
+      <c r="G51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43513</v>
       </c>
@@ -1772,8 +1832,14 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>14</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43514</v>
       </c>
@@ -1793,8 +1859,14 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>12</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43515</v>
       </c>
@@ -1814,8 +1886,14 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>8</v>
+      </c>
+      <c r="G54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43516</v>
       </c>
@@ -1835,8 +1913,14 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43517</v>
       </c>
@@ -1856,8 +1940,14 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>18</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43518</v>
       </c>
@@ -1877,8 +1967,14 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>17</v>
+      </c>
+      <c r="G57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43519</v>
       </c>
@@ -1898,8 +1994,14 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43520</v>
       </c>
@@ -1919,8 +2021,14 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>4</v>
+      </c>
+      <c r="G59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43521</v>
       </c>
@@ -1940,8 +2048,14 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>9</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43522</v>
       </c>
@@ -1961,8 +2075,14 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <v>20</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43523</v>
       </c>
@@ -1982,8 +2102,14 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>5</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43524</v>
       </c>
@@ -2003,8 +2129,14 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>36</v>
+      </c>
+      <c r="G63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43525</v>
       </c>
@@ -2024,8 +2156,14 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>43526</v>
       </c>
@@ -2045,8 +2183,14 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>43527</v>
       </c>
@@ -2066,8 +2210,14 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <v>8</v>
+      </c>
+      <c r="G66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>43528</v>
       </c>
@@ -2087,8 +2237,14 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>20</v>
+      </c>
+      <c r="G67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>43529</v>
       </c>
@@ -2109,7 +2265,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>43530</v>
       </c>
@@ -2130,7 +2286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>43531</v>
       </c>
@@ -2151,7 +2307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>43532</v>
       </c>
@@ -2172,7 +2328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>43533</v>
       </c>
@@ -2193,7 +2349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>43534</v>
       </c>
@@ -2214,7 +2370,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>43535</v>
       </c>
@@ -2235,7 +2391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>43536</v>
       </c>
@@ -2256,7 +2412,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>43537</v>
       </c>
@@ -2277,7 +2433,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>43538</v>
       </c>
@@ -2298,7 +2454,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>43539</v>
       </c>
@@ -2319,7 +2475,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>43540</v>
       </c>
@@ -2340,7 +2496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>43541</v>
       </c>

</xml_diff>

<commit_message>
updating my reads and adding pkane goal data
</commit_message>
<xml_diff>
--- a/data/my-reads.xlsx
+++ b/data/my-reads.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Desktop/github-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843BB512-0CB6-1F48-8401-50D6FB63EF7E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CF8A86-01DB-1B4D-B418-1391969E02B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{6A43893A-E979-8943-8C08-0CBFF629ACEC}"/>
   </bookViews>
@@ -435,8 +435,8 @@
   <dimension ref="A1:G369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G77" sqref="G77"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G76" sqref="G76:G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2509,6 +2509,12 @@
         <f t="shared" si="15"/>
         <v>11</v>
       </c>
+      <c r="F77">
+        <v>6</v>
+      </c>
+      <c r="G77">
+        <v>3</v>
+      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
@@ -2530,6 +2536,12 @@
         <f t="shared" si="15"/>
         <v>11</v>
       </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>3</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
@@ -2551,6 +2563,12 @@
         <f t="shared" si="15"/>
         <v>11</v>
       </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>3</v>
+      </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
@@ -2572,8 +2590,14 @@
         <f t="shared" si="15"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <v>2</v>
+      </c>
+      <c r="G80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43542</v>
       </c>
@@ -2593,8 +2617,14 @@
         <f t="shared" si="15"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <v>6</v>
+      </c>
+      <c r="G81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>43543</v>
       </c>
@@ -2614,8 +2644,14 @@
         <f t="shared" si="15"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>43544</v>
       </c>
@@ -2635,8 +2671,14 @@
         <f t="shared" si="15"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>43545</v>
       </c>
@@ -2656,8 +2698,14 @@
         <f t="shared" si="15"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>43546</v>
       </c>
@@ -2677,8 +2725,14 @@
         <f t="shared" si="15"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>43547</v>
       </c>
@@ -2698,8 +2752,14 @@
         <f t="shared" si="15"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <v>5</v>
+      </c>
+      <c r="G86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>43548</v>
       </c>
@@ -2719,8 +2779,14 @@
         <f t="shared" si="15"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>43549</v>
       </c>
@@ -2740,8 +2806,14 @@
         <f t="shared" si="15"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>43550</v>
       </c>
@@ -2761,8 +2833,14 @@
         <f t="shared" si="15"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <v>5</v>
+      </c>
+      <c r="G89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>43551</v>
       </c>
@@ -2782,8 +2860,14 @@
         <f t="shared" si="15"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>43552</v>
       </c>
@@ -2803,8 +2887,14 @@
         <f t="shared" si="15"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <v>8</v>
+      </c>
+      <c r="G91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>43553</v>
       </c>
@@ -2824,8 +2914,14 @@
         <f t="shared" si="15"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>43554</v>
       </c>
@@ -2845,8 +2941,14 @@
         <f t="shared" si="15"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>43555</v>
       </c>
@@ -2866,8 +2968,14 @@
         <f t="shared" si="15"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>43556</v>
       </c>
@@ -2887,8 +2995,14 @@
         <f t="shared" si="15"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <v>5</v>
+      </c>
+      <c r="G95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>43557</v>
       </c>

</xml_diff>

<commit_message>
updating my-reads to add correct book #4
</commit_message>
<xml_diff>
--- a/data/my-reads.xlsx
+++ b/data/my-reads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Desktop/github-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CF8A86-01DB-1B4D-B418-1391969E02B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463B81A5-5578-B146-9E64-E582A9975CC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{6A43893A-E979-8943-8C08-0CBFF629ACEC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>Mike X Cohen</t>
+  </si>
+  <si>
+    <t>The Sensory Order</t>
+  </si>
+  <si>
+    <t>Friedrich A. Hayek</t>
   </si>
 </sst>
 </file>
@@ -435,8 +441,8 @@
   <dimension ref="A1:G369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G76" sqref="G76:G95"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G72" sqref="G72:G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2351,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="G71">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -2378,7 +2384,7 @@
         <v>0</v>
       </c>
       <c r="G72">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -2405,7 +2411,7 @@
         <v>13</v>
       </c>
       <c r="G73">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -2432,7 +2438,7 @@
         <v>0</v>
       </c>
       <c r="G74">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -2459,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="G75">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -2486,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="G76">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -2513,7 +2519,7 @@
         <v>6</v>
       </c>
       <c r="G77">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -2540,7 +2546,7 @@
         <v>0</v>
       </c>
       <c r="G78">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -2567,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="G79">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -2594,7 +2600,7 @@
         <v>2</v>
       </c>
       <c r="G80">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -2621,7 +2627,7 @@
         <v>6</v>
       </c>
       <c r="G81">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -2648,7 +2654,7 @@
         <v>0</v>
       </c>
       <c r="G82">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -2675,7 +2681,7 @@
         <v>0</v>
       </c>
       <c r="G83">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -2702,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="G84">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -2729,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="G85">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -2756,7 +2762,7 @@
         <v>5</v>
       </c>
       <c r="G86">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -2783,7 +2789,7 @@
         <v>0</v>
       </c>
       <c r="G87">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -2810,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="G88">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -2837,7 +2843,7 @@
         <v>5</v>
       </c>
       <c r="G89">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -2864,7 +2870,7 @@
         <v>0</v>
       </c>
       <c r="G90">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -2891,7 +2897,7 @@
         <v>8</v>
       </c>
       <c r="G91">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -2918,7 +2924,7 @@
         <v>0</v>
       </c>
       <c r="G92">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -2945,7 +2951,7 @@
         <v>0</v>
       </c>
       <c r="G93">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -2972,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="G94">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -2999,7 +3005,7 @@
         <v>5</v>
       </c>
       <c r="G95">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -8763,7 +8769,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082B48B6-1501-774C-818C-F75B39B01AEE}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -8832,6 +8838,20 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>1952</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated my reads' data for aug + sep 2019
</commit_message>
<xml_diff>
--- a/data/my-reads.xlsx
+++ b/data/my-reads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjk140130/Desktop/githup-repos/github-website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Desktop/githup-repos/github-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1247EE12-574F-9743-8C68-3ECB809C0DEE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776E2B5E-4365-3048-9FD4-B8F1EC42BAA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25680" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{6A43893A-E979-8943-8C08-0CBFF629ACEC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{6A43893A-E979-8943-8C08-0CBFF629ACEC}"/>
   </bookViews>
   <sheets>
     <sheet name="reading-data" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>date</t>
   </si>
@@ -115,6 +116,12 @@
   </si>
   <si>
     <t>D. O. Hebb</t>
+  </si>
+  <si>
+    <t>The Disordered Mind</t>
+  </si>
+  <si>
+    <t>Eric R. Kandel</t>
   </si>
 </sst>
 </file>
@@ -467,11 +474,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F081B7-288B-1045-AB76-1CD03FBCB65E}">
-  <dimension ref="A1:G370"/>
+  <dimension ref="A1:G373"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F232" sqref="F232"/>
+      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H293" sqref="H293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5850,19 +5857,19 @@
         <v>43661</v>
       </c>
       <c r="B200">
-        <f t="shared" ref="B200:B264" si="20">YEAR(A200)</f>
+        <f t="shared" ref="B200:B267" si="20">YEAR(A200)</f>
         <v>2019</v>
       </c>
       <c r="C200">
-        <f t="shared" ref="C200:C264" si="21">MONTH(A200)</f>
+        <f t="shared" ref="C200:C267" si="21">MONTH(A200)</f>
         <v>7</v>
       </c>
       <c r="D200">
-        <f t="shared" ref="D200:D264" si="22">DAY(A200)</f>
+        <f t="shared" ref="D200:D267" si="22">DAY(A200)</f>
         <v>15</v>
       </c>
       <c r="E200">
-        <f t="shared" ref="E200:E264" si="23">WEEKNUM(A200)</f>
+        <f t="shared" ref="E200:E267" si="23">WEEKNUM(A200)</f>
         <v>29</v>
       </c>
       <c r="F200">
@@ -6738,112 +6745,142 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
+        <v>43692</v>
+      </c>
+      <c r="B233">
+        <f t="shared" ref="B233" si="28">YEAR(A233)</f>
+        <v>2019</v>
+      </c>
+      <c r="C233">
+        <f t="shared" ref="C233" si="29">MONTH(A233)</f>
+        <v>8</v>
+      </c>
+      <c r="D233">
+        <f t="shared" ref="D233" si="30">DAY(A233)</f>
+        <v>15</v>
+      </c>
+      <c r="E233">
+        <f t="shared" ref="E233" si="31">WEEKNUM(A233)</f>
+        <v>33</v>
+      </c>
+      <c r="F233">
+        <v>17</v>
+      </c>
+      <c r="G233">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A234" s="1">
         <v>43693</v>
       </c>
-      <c r="B233">
+      <c r="B234">
         <f t="shared" si="20"/>
         <v>2019</v>
       </c>
-      <c r="C233">
+      <c r="C234">
         <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="D233">
+      <c r="D234">
         <f t="shared" si="22"/>
         <v>16</v>
-      </c>
-      <c r="E233">
-        <f t="shared" si="23"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A234" s="1">
-        <v>43694</v>
-      </c>
-      <c r="B234">
-        <f t="shared" si="20"/>
-        <v>2019</v>
-      </c>
-      <c r="C234">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
-      <c r="D234">
-        <f t="shared" si="22"/>
-        <v>17</v>
       </c>
       <c r="E234">
         <f t="shared" si="23"/>
         <v>33</v>
       </c>
+      <c r="F234">
+        <v>0</v>
+      </c>
+      <c r="G234">
+        <v>8</v>
+      </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
+        <v>43693</v>
+      </c>
+      <c r="B235">
+        <f t="shared" ref="B235" si="32">YEAR(A235)</f>
+        <v>2019</v>
+      </c>
+      <c r="C235">
+        <f t="shared" ref="C235" si="33">MONTH(A235)</f>
+        <v>8</v>
+      </c>
+      <c r="D235">
+        <f t="shared" ref="D235" si="34">DAY(A235)</f>
+        <v>16</v>
+      </c>
+      <c r="E235">
+        <f t="shared" ref="E235" si="35">WEEKNUM(A235)</f>
+        <v>33</v>
+      </c>
+      <c r="F235">
+        <v>13</v>
+      </c>
+      <c r="G235">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A236" s="1">
+        <v>43694</v>
+      </c>
+      <c r="B236">
+        <f t="shared" si="20"/>
+        <v>2019</v>
+      </c>
+      <c r="C236">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="D236">
+        <f t="shared" si="22"/>
+        <v>17</v>
+      </c>
+      <c r="E236">
+        <f t="shared" si="23"/>
+        <v>33</v>
+      </c>
+      <c r="F236">
+        <v>12</v>
+      </c>
+      <c r="G236">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A237" s="1">
         <v>43695</v>
       </c>
-      <c r="B235">
+      <c r="B237">
         <f t="shared" si="20"/>
         <v>2019</v>
       </c>
-      <c r="C235">
+      <c r="C237">
         <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="D235">
+      <c r="D237">
         <f t="shared" si="22"/>
         <v>18</v>
-      </c>
-      <c r="E235">
-        <f t="shared" si="23"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A236" s="1">
-        <v>43696</v>
-      </c>
-      <c r="B236">
-        <f t="shared" si="20"/>
-        <v>2019</v>
-      </c>
-      <c r="C236">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
-      <c r="D236">
-        <f t="shared" si="22"/>
-        <v>19</v>
-      </c>
-      <c r="E236">
-        <f t="shared" si="23"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A237" s="1">
-        <v>43697</v>
-      </c>
-      <c r="B237">
-        <f t="shared" si="20"/>
-        <v>2019</v>
-      </c>
-      <c r="C237">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
-      <c r="D237">
-        <f t="shared" si="22"/>
-        <v>20</v>
       </c>
       <c r="E237">
         <f t="shared" si="23"/>
         <v>34</v>
       </c>
+      <c r="F237">
+        <v>41</v>
+      </c>
+      <c r="G237">
+        <v>8</v>
+      </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
-        <v>43698</v>
+        <v>43696</v>
       </c>
       <c r="B238">
         <f t="shared" si="20"/>
@@ -6855,37 +6892,49 @@
       </c>
       <c r="D238">
         <f t="shared" si="22"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E238">
         <f t="shared" si="23"/>
         <v>34</v>
       </c>
+      <c r="F238">
+        <v>15</v>
+      </c>
+      <c r="G238">
+        <v>8</v>
+      </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
-        <v>43699</v>
+        <v>43696</v>
       </c>
       <c r="B239">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="B239" si="36">YEAR(A239)</f>
         <v>2019</v>
       </c>
       <c r="C239">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="C239" si="37">MONTH(A239)</f>
         <v>8</v>
       </c>
       <c r="D239">
-        <f t="shared" si="22"/>
-        <v>22</v>
+        <f t="shared" ref="D239" si="38">DAY(A239)</f>
+        <v>19</v>
       </c>
       <c r="E239">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="E239" si="39">WEEKNUM(A239)</f>
         <v>34</v>
+      </c>
+      <c r="F239">
+        <v>9</v>
+      </c>
+      <c r="G239">
+        <v>9</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
-        <v>43700</v>
+        <v>43697</v>
       </c>
       <c r="B240">
         <f t="shared" si="20"/>
@@ -6897,16 +6946,22 @@
       </c>
       <c r="D240">
         <f t="shared" si="22"/>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E240">
         <f t="shared" si="23"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F240">
+        <v>16</v>
+      </c>
+      <c r="G240">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
-        <v>43701</v>
+        <v>43698</v>
       </c>
       <c r="B241">
         <f t="shared" si="20"/>
@@ -6918,16 +6973,22 @@
       </c>
       <c r="D241">
         <f t="shared" si="22"/>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E241">
         <f t="shared" si="23"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F241">
+        <v>8</v>
+      </c>
+      <c r="G241">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
-        <v>43702</v>
+        <v>43699</v>
       </c>
       <c r="B242">
         <f t="shared" si="20"/>
@@ -6939,16 +7000,22 @@
       </c>
       <c r="D242">
         <f t="shared" si="22"/>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E242">
         <f t="shared" si="23"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="F242">
+        <v>10</v>
+      </c>
+      <c r="G242">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
-        <v>43703</v>
+        <v>43700</v>
       </c>
       <c r="B243">
         <f t="shared" si="20"/>
@@ -6960,16 +7027,22 @@
       </c>
       <c r="D243">
         <f t="shared" si="22"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E243">
         <f t="shared" si="23"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="F243">
+        <v>0</v>
+      </c>
+      <c r="G243">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
-        <v>43704</v>
+        <v>43701</v>
       </c>
       <c r="B244">
         <f t="shared" si="20"/>
@@ -6981,16 +7054,22 @@
       </c>
       <c r="D244">
         <f t="shared" si="22"/>
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E244">
         <f t="shared" si="23"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="F244">
+        <v>10</v>
+      </c>
+      <c r="G244">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
-        <v>43705</v>
+        <v>43702</v>
       </c>
       <c r="B245">
         <f t="shared" si="20"/>
@@ -7002,16 +7081,22 @@
       </c>
       <c r="D245">
         <f t="shared" si="22"/>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E245">
         <f t="shared" si="23"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F245">
+        <v>6</v>
+      </c>
+      <c r="G245">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
-        <v>43706</v>
+        <v>43703</v>
       </c>
       <c r="B246">
         <f t="shared" si="20"/>
@@ -7023,16 +7108,22 @@
       </c>
       <c r="D246">
         <f t="shared" si="22"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E246">
         <f t="shared" si="23"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F246">
+        <v>14</v>
+      </c>
+      <c r="G246">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
-        <v>43707</v>
+        <v>43704</v>
       </c>
       <c r="B247">
         <f t="shared" si="20"/>
@@ -7044,16 +7135,22 @@
       </c>
       <c r="D247">
         <f t="shared" si="22"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E247">
         <f t="shared" si="23"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F247">
+        <v>13</v>
+      </c>
+      <c r="G247">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
-        <v>43708</v>
+        <v>43705</v>
       </c>
       <c r="B248">
         <f t="shared" si="20"/>
@@ -7065,16 +7162,22 @@
       </c>
       <c r="D248">
         <f t="shared" si="22"/>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E248">
         <f t="shared" si="23"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F248">
+        <v>11</v>
+      </c>
+      <c r="G248">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
-        <v>43709</v>
+        <v>43706</v>
       </c>
       <c r="B249">
         <f t="shared" si="20"/>
@@ -7082,20 +7185,26 @@
       </c>
       <c r="C249">
         <f t="shared" si="21"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D249">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E249">
         <f t="shared" si="23"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="F249">
+        <v>0</v>
+      </c>
+      <c r="G249">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
-        <v>43710</v>
+        <v>43707</v>
       </c>
       <c r="B250">
         <f t="shared" si="20"/>
@@ -7103,20 +7212,26 @@
       </c>
       <c r="C250">
         <f t="shared" si="21"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D250">
         <f t="shared" si="22"/>
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E250">
         <f t="shared" si="23"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="F250">
+        <v>0</v>
+      </c>
+      <c r="G250">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
-        <v>43711</v>
+        <v>43708</v>
       </c>
       <c r="B251">
         <f t="shared" si="20"/>
@@ -7124,20 +7239,26 @@
       </c>
       <c r="C251">
         <f t="shared" si="21"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D251">
         <f t="shared" si="22"/>
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E251">
         <f t="shared" si="23"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="F251">
+        <v>14</v>
+      </c>
+      <c r="G251">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
-        <v>43712</v>
+        <v>43709</v>
       </c>
       <c r="B252">
         <f t="shared" si="20"/>
@@ -7149,16 +7270,22 @@
       </c>
       <c r="D252">
         <f t="shared" si="22"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E252">
         <f t="shared" si="23"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F252">
+        <v>0</v>
+      </c>
+      <c r="G252">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
-        <v>43713</v>
+        <v>43710</v>
       </c>
       <c r="B253">
         <f t="shared" si="20"/>
@@ -7170,16 +7297,22 @@
       </c>
       <c r="D253">
         <f t="shared" si="22"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E253">
         <f t="shared" si="23"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F253">
+        <v>0</v>
+      </c>
+      <c r="G253">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
-        <v>43714</v>
+        <v>43711</v>
       </c>
       <c r="B254">
         <f t="shared" si="20"/>
@@ -7191,16 +7324,22 @@
       </c>
       <c r="D254">
         <f t="shared" si="22"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E254">
         <f t="shared" si="23"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F254">
+        <v>0</v>
+      </c>
+      <c r="G254">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
-        <v>43715</v>
+        <v>43712</v>
       </c>
       <c r="B255">
         <f t="shared" si="20"/>
@@ -7212,16 +7351,22 @@
       </c>
       <c r="D255">
         <f t="shared" si="22"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E255">
         <f t="shared" si="23"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F255">
+        <v>6</v>
+      </c>
+      <c r="G255">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="B256">
         <f t="shared" si="20"/>
@@ -7233,16 +7378,22 @@
       </c>
       <c r="D256">
         <f t="shared" si="22"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E256">
         <f t="shared" si="23"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="F256">
+        <v>0</v>
+      </c>
+      <c r="G256">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
-        <v>43717</v>
+        <v>43714</v>
       </c>
       <c r="B257">
         <f t="shared" si="20"/>
@@ -7254,16 +7405,22 @@
       </c>
       <c r="D257">
         <f t="shared" si="22"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E257">
         <f t="shared" si="23"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="F257">
+        <v>0</v>
+      </c>
+      <c r="G257">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
-        <v>43718</v>
+        <v>43715</v>
       </c>
       <c r="B258">
         <f t="shared" si="20"/>
@@ -7275,16 +7432,22 @@
       </c>
       <c r="D258">
         <f t="shared" si="22"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E258">
         <f t="shared" si="23"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="F258">
+        <v>0</v>
+      </c>
+      <c r="G258">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
-        <v>43719</v>
+        <v>43716</v>
       </c>
       <c r="B259">
         <f t="shared" si="20"/>
@@ -7296,16 +7459,22 @@
       </c>
       <c r="D259">
         <f t="shared" si="22"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E259">
         <f t="shared" si="23"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F259">
+        <v>0</v>
+      </c>
+      <c r="G259">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
-        <v>43720</v>
+        <v>43717</v>
       </c>
       <c r="B260">
         <f t="shared" si="20"/>
@@ -7317,16 +7486,22 @@
       </c>
       <c r="D260">
         <f t="shared" si="22"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E260">
         <f t="shared" si="23"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F260">
+        <v>0</v>
+      </c>
+      <c r="G260">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
-        <v>43721</v>
+        <v>43718</v>
       </c>
       <c r="B261">
         <f t="shared" si="20"/>
@@ -7338,16 +7513,22 @@
       </c>
       <c r="D261">
         <f t="shared" si="22"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E261">
         <f t="shared" si="23"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F261">
+        <v>0</v>
+      </c>
+      <c r="G261">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
-        <v>43722</v>
+        <v>43719</v>
       </c>
       <c r="B262">
         <f t="shared" si="20"/>
@@ -7359,16 +7540,22 @@
       </c>
       <c r="D262">
         <f t="shared" si="22"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E262">
         <f t="shared" si="23"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F262">
+        <v>8</v>
+      </c>
+      <c r="G262">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
-        <v>43723</v>
+        <v>43720</v>
       </c>
       <c r="B263">
         <f t="shared" si="20"/>
@@ -7380,16 +7567,22 @@
       </c>
       <c r="D263">
         <f t="shared" si="22"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E263">
         <f t="shared" si="23"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="F263">
+        <v>0</v>
+      </c>
+      <c r="G263">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
-        <v>43724</v>
+        <v>43721</v>
       </c>
       <c r="B264">
         <f t="shared" si="20"/>
@@ -7401,2236 +7594,2461 @@
       </c>
       <c r="D264">
         <f t="shared" si="22"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E264">
         <f t="shared" si="23"/>
+        <v>37</v>
+      </c>
+      <c r="F264">
+        <v>0</v>
+      </c>
+      <c r="G264">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A265" s="1">
+        <v>43722</v>
+      </c>
+      <c r="B265">
+        <f t="shared" si="20"/>
+        <v>2019</v>
+      </c>
+      <c r="C265">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="D265">
+        <f t="shared" si="22"/>
+        <v>14</v>
+      </c>
+      <c r="E265">
+        <f t="shared" si="23"/>
+        <v>37</v>
+      </c>
+      <c r="F265">
+        <v>0</v>
+      </c>
+      <c r="G265">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A266" s="1">
+        <v>43723</v>
+      </c>
+      <c r="B266">
+        <f t="shared" si="20"/>
+        <v>2019</v>
+      </c>
+      <c r="C266">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="D266">
+        <f t="shared" si="22"/>
+        <v>15</v>
+      </c>
+      <c r="E266">
+        <f t="shared" si="23"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A265" s="1">
+      <c r="F266">
+        <v>0</v>
+      </c>
+      <c r="G266">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A267" s="1">
+        <v>43724</v>
+      </c>
+      <c r="B267">
+        <f t="shared" si="20"/>
+        <v>2019</v>
+      </c>
+      <c r="C267">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="D267">
+        <f t="shared" si="22"/>
+        <v>16</v>
+      </c>
+      <c r="E267">
+        <f t="shared" si="23"/>
+        <v>38</v>
+      </c>
+      <c r="F267">
+        <v>0</v>
+      </c>
+      <c r="G267">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A268" s="1">
         <v>43725</v>
       </c>
-      <c r="B265">
-        <f t="shared" ref="B265:B328" si="28">YEAR(A265)</f>
-        <v>2019</v>
-      </c>
-      <c r="C265">
-        <f t="shared" ref="C265:C328" si="29">MONTH(A265)</f>
+      <c r="B268">
+        <f t="shared" ref="B268:B331" si="40">YEAR(A268)</f>
+        <v>2019</v>
+      </c>
+      <c r="C268">
+        <f t="shared" ref="C268:C331" si="41">MONTH(A268)</f>
         <v>9</v>
       </c>
-      <c r="D265">
-        <f t="shared" ref="D265:D328" si="30">DAY(A265)</f>
+      <c r="D268">
+        <f t="shared" ref="D268:D331" si="42">DAY(A268)</f>
         <v>17</v>
       </c>
-      <c r="E265">
-        <f t="shared" ref="E265:E328" si="31">WEEKNUM(A265)</f>
+      <c r="E268">
+        <f t="shared" ref="E268:E331" si="43">WEEKNUM(A268)</f>
         <v>38</v>
       </c>
-    </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A266" s="1">
+      <c r="F268">
+        <v>0</v>
+      </c>
+      <c r="G268">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A269" s="1">
         <v>43726</v>
       </c>
-      <c r="B266">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C266">
-        <f t="shared" si="29"/>
+      <c r="B269">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C269">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D266">
-        <f t="shared" si="30"/>
+      <c r="D269">
+        <f t="shared" si="42"/>
         <v>18</v>
       </c>
-      <c r="E266">
-        <f t="shared" si="31"/>
+      <c r="E269">
+        <f t="shared" si="43"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A267" s="1">
+      <c r="F269">
+        <v>0</v>
+      </c>
+      <c r="G269">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A270" s="1">
         <v>43727</v>
       </c>
-      <c r="B267">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C267">
-        <f t="shared" si="29"/>
+      <c r="B270">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C270">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D267">
-        <f t="shared" si="30"/>
+      <c r="D270">
+        <f t="shared" si="42"/>
         <v>19</v>
       </c>
-      <c r="E267">
-        <f t="shared" si="31"/>
+      <c r="E270">
+        <f t="shared" si="43"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A268" s="1">
+      <c r="F270">
+        <v>0</v>
+      </c>
+      <c r="G270">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A271" s="1">
         <v>43728</v>
       </c>
-      <c r="B268">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C268">
-        <f t="shared" si="29"/>
+      <c r="B271">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C271">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D268">
-        <f t="shared" si="30"/>
+      <c r="D271">
+        <f t="shared" si="42"/>
         <v>20</v>
       </c>
-      <c r="E268">
-        <f t="shared" si="31"/>
+      <c r="E271">
+        <f t="shared" si="43"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A269" s="1">
+      <c r="F271">
+        <v>0</v>
+      </c>
+      <c r="G271">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A272" s="1">
         <v>43729</v>
       </c>
-      <c r="B269">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C269">
-        <f t="shared" si="29"/>
+      <c r="B272">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C272">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D269">
-        <f t="shared" si="30"/>
+      <c r="D272">
+        <f t="shared" si="42"/>
         <v>21</v>
       </c>
-      <c r="E269">
-        <f t="shared" si="31"/>
+      <c r="E272">
+        <f t="shared" si="43"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A270" s="1">
+      <c r="F272">
+        <v>0</v>
+      </c>
+      <c r="G272">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A273" s="1">
         <v>43730</v>
       </c>
-      <c r="B270">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C270">
-        <f t="shared" si="29"/>
+      <c r="B273">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C273">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D270">
-        <f t="shared" si="30"/>
+      <c r="D273">
+        <f t="shared" si="42"/>
         <v>22</v>
       </c>
-      <c r="E270">
-        <f t="shared" si="31"/>
+      <c r="E273">
+        <f t="shared" si="43"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A271" s="1">
+      <c r="F273">
+        <v>0</v>
+      </c>
+      <c r="G273">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A274" s="1">
         <v>43731</v>
       </c>
-      <c r="B271">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C271">
-        <f t="shared" si="29"/>
+      <c r="B274">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C274">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D271">
-        <f t="shared" si="30"/>
+      <c r="D274">
+        <f t="shared" si="42"/>
         <v>23</v>
       </c>
-      <c r="E271">
-        <f t="shared" si="31"/>
+      <c r="E274">
+        <f t="shared" si="43"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A272" s="1">
+      <c r="F274">
+        <v>6</v>
+      </c>
+      <c r="G274">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A275" s="1">
         <v>43732</v>
       </c>
-      <c r="B272">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C272">
-        <f t="shared" si="29"/>
+      <c r="B275">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C275">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D272">
-        <f t="shared" si="30"/>
+      <c r="D275">
+        <f t="shared" si="42"/>
         <v>24</v>
       </c>
-      <c r="E272">
-        <f t="shared" si="31"/>
+      <c r="E275">
+        <f t="shared" si="43"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A273" s="1">
+      <c r="F275">
+        <v>2</v>
+      </c>
+      <c r="G275">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A276" s="1">
         <v>43733</v>
       </c>
-      <c r="B273">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C273">
-        <f t="shared" si="29"/>
+      <c r="B276">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C276">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D273">
-        <f t="shared" si="30"/>
+      <c r="D276">
+        <f t="shared" si="42"/>
         <v>25</v>
       </c>
-      <c r="E273">
-        <f t="shared" si="31"/>
+      <c r="E276">
+        <f t="shared" si="43"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A274" s="1">
+      <c r="F276">
+        <v>11</v>
+      </c>
+      <c r="G276">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A277" s="1">
         <v>43734</v>
       </c>
-      <c r="B274">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C274">
-        <f t="shared" si="29"/>
+      <c r="B277">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C277">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D274">
-        <f t="shared" si="30"/>
+      <c r="D277">
+        <f t="shared" si="42"/>
         <v>26</v>
       </c>
-      <c r="E274">
-        <f t="shared" si="31"/>
+      <c r="E277">
+        <f t="shared" si="43"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A275" s="1">
+      <c r="F277">
+        <v>0</v>
+      </c>
+      <c r="G277">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A278" s="1">
         <v>43735</v>
       </c>
-      <c r="B275">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C275">
-        <f t="shared" si="29"/>
+      <c r="B278">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C278">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D275">
-        <f t="shared" si="30"/>
+      <c r="D278">
+        <f t="shared" si="42"/>
         <v>27</v>
       </c>
-      <c r="E275">
-        <f t="shared" si="31"/>
+      <c r="E278">
+        <f t="shared" si="43"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A276" s="1">
+      <c r="F278">
+        <v>0</v>
+      </c>
+      <c r="G278">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A279" s="1">
         <v>43736</v>
       </c>
-      <c r="B276">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C276">
-        <f t="shared" si="29"/>
+      <c r="B279">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C279">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D276">
-        <f t="shared" si="30"/>
+      <c r="D279">
+        <f t="shared" si="42"/>
         <v>28</v>
       </c>
-      <c r="E276">
-        <f t="shared" si="31"/>
+      <c r="E279">
+        <f t="shared" si="43"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A277" s="1">
+      <c r="F279">
+        <v>0</v>
+      </c>
+      <c r="G279">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A280" s="1">
         <v>43737</v>
       </c>
-      <c r="B277">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C277">
-        <f t="shared" si="29"/>
+      <c r="B280">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C280">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D277">
-        <f t="shared" si="30"/>
+      <c r="D280">
+        <f t="shared" si="42"/>
         <v>29</v>
       </c>
-      <c r="E277">
-        <f t="shared" si="31"/>
+      <c r="E280">
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A278" s="1">
+      <c r="F280">
+        <v>5</v>
+      </c>
+      <c r="G280">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A281" s="1">
         <v>43738</v>
       </c>
-      <c r="B278">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C278">
-        <f t="shared" si="29"/>
+      <c r="B281">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C281">
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
-      <c r="D278">
-        <f t="shared" si="30"/>
+      <c r="D281">
+        <f t="shared" si="42"/>
         <v>30</v>
       </c>
-      <c r="E278">
-        <f t="shared" si="31"/>
+      <c r="E281">
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A279" s="1">
+      <c r="F281">
+        <v>8</v>
+      </c>
+      <c r="G281">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A282" s="1">
         <v>43739</v>
       </c>
-      <c r="B279">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C279">
-        <f t="shared" si="29"/>
+      <c r="B282">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C282">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D279">
-        <f t="shared" si="30"/>
+      <c r="D282">
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
-      <c r="E279">
-        <f t="shared" si="31"/>
+      <c r="E282">
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A280" s="1">
+      <c r="F282">
+        <v>16</v>
+      </c>
+      <c r="G282">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A283" s="1">
         <v>43740</v>
       </c>
-      <c r="B280">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C280">
-        <f t="shared" si="29"/>
+      <c r="B283">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C283">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D280">
-        <f t="shared" si="30"/>
+      <c r="D283">
+        <f t="shared" si="42"/>
         <v>2</v>
       </c>
-      <c r="E280">
-        <f t="shared" si="31"/>
+      <c r="E283">
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A281" s="1">
+      <c r="F283">
+        <v>0</v>
+      </c>
+      <c r="G283">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A284" s="1">
         <v>43741</v>
       </c>
-      <c r="B281">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C281">
-        <f t="shared" si="29"/>
+      <c r="B284">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C284">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D281">
-        <f t="shared" si="30"/>
+      <c r="D284">
+        <f t="shared" si="42"/>
         <v>3</v>
       </c>
-      <c r="E281">
-        <f t="shared" si="31"/>
+      <c r="E284">
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A282" s="1">
+      <c r="F284">
+        <v>0</v>
+      </c>
+      <c r="G284">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A285" s="1">
         <v>43742</v>
       </c>
-      <c r="B282">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C282">
-        <f t="shared" si="29"/>
+      <c r="B285">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C285">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D282">
-        <f t="shared" si="30"/>
-        <v>4</v>
-      </c>
-      <c r="E282">
-        <f t="shared" si="31"/>
+      <c r="D285">
+        <f t="shared" si="42"/>
+        <v>4</v>
+      </c>
+      <c r="E285">
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A283" s="1">
+      <c r="F285">
+        <v>0</v>
+      </c>
+      <c r="G285">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A286" s="1">
         <v>43743</v>
       </c>
-      <c r="B283">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C283">
-        <f t="shared" si="29"/>
+      <c r="B286">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C286">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D283">
-        <f t="shared" si="30"/>
+      <c r="D286">
+        <f t="shared" si="42"/>
         <v>5</v>
       </c>
-      <c r="E283">
-        <f t="shared" si="31"/>
+      <c r="E286">
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A284" s="1">
+      <c r="F286">
+        <v>0</v>
+      </c>
+      <c r="G286">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A287" s="1">
         <v>43744</v>
       </c>
-      <c r="B284">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C284">
-        <f t="shared" si="29"/>
+      <c r="B287">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C287">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D284">
-        <f t="shared" si="30"/>
+      <c r="D287">
+        <f t="shared" si="42"/>
         <v>6</v>
       </c>
-      <c r="E284">
-        <f t="shared" si="31"/>
+      <c r="E287">
+        <f t="shared" si="43"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A285" s="1">
+      <c r="F287">
+        <v>0</v>
+      </c>
+      <c r="G287">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A288" s="1">
         <v>43745</v>
       </c>
-      <c r="B285">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C285">
-        <f t="shared" si="29"/>
+      <c r="B288">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C288">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D285">
-        <f t="shared" si="30"/>
+      <c r="D288">
+        <f t="shared" si="42"/>
         <v>7</v>
       </c>
-      <c r="E285">
-        <f t="shared" si="31"/>
+      <c r="E288">
+        <f t="shared" si="43"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A286" s="1">
+      <c r="F288">
+        <v>0</v>
+      </c>
+      <c r="G288">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A289" s="1">
         <v>43746</v>
       </c>
-      <c r="B286">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C286">
-        <f t="shared" si="29"/>
+      <c r="B289">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C289">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D286">
-        <f t="shared" si="30"/>
-        <v>8</v>
-      </c>
-      <c r="E286">
-        <f t="shared" si="31"/>
+      <c r="D289">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E289">
+        <f t="shared" si="43"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A287" s="1">
+      <c r="F289">
+        <v>14</v>
+      </c>
+      <c r="G289">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A290" s="1">
         <v>43747</v>
       </c>
-      <c r="B287">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C287">
-        <f t="shared" si="29"/>
+      <c r="B290">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C290">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D287">
-        <f t="shared" si="30"/>
+      <c r="D290">
+        <f t="shared" si="42"/>
         <v>9</v>
       </c>
-      <c r="E287">
-        <f t="shared" si="31"/>
+      <c r="E290">
+        <f t="shared" si="43"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A288" s="1">
+      <c r="F290">
+        <v>8</v>
+      </c>
+      <c r="G290">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A291" s="1">
         <v>43748</v>
       </c>
-      <c r="B288">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C288">
-        <f t="shared" si="29"/>
+      <c r="B291">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C291">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D288">
-        <f t="shared" si="30"/>
+      <c r="D291">
+        <f t="shared" si="42"/>
         <v>10</v>
       </c>
-      <c r="E288">
-        <f t="shared" si="31"/>
+      <c r="E291">
+        <f t="shared" si="43"/>
         <v>41</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A289" s="1">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A292" s="1">
         <v>43749</v>
       </c>
-      <c r="B289">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C289">
-        <f t="shared" si="29"/>
+      <c r="B292">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C292">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D289">
-        <f t="shared" si="30"/>
+      <c r="D292">
+        <f t="shared" si="42"/>
         <v>11</v>
       </c>
-      <c r="E289">
-        <f t="shared" si="31"/>
+      <c r="E292">
+        <f t="shared" si="43"/>
         <v>41</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A290" s="1">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A293" s="1">
         <v>43750</v>
       </c>
-      <c r="B290">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C290">
-        <f t="shared" si="29"/>
+      <c r="B293">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C293">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D290">
-        <f t="shared" si="30"/>
+      <c r="D293">
+        <f t="shared" si="42"/>
         <v>12</v>
       </c>
-      <c r="E290">
-        <f t="shared" si="31"/>
+      <c r="E293">
+        <f t="shared" si="43"/>
         <v>41</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A291" s="1">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A294" s="1">
         <v>43751</v>
       </c>
-      <c r="B291">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C291">
-        <f t="shared" si="29"/>
+      <c r="B294">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C294">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D291">
-        <f t="shared" si="30"/>
+      <c r="D294">
+        <f t="shared" si="42"/>
         <v>13</v>
       </c>
-      <c r="E291">
-        <f t="shared" si="31"/>
+      <c r="E294">
+        <f t="shared" si="43"/>
         <v>42</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A292" s="1">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A295" s="1">
         <v>43752</v>
       </c>
-      <c r="B292">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C292">
-        <f t="shared" si="29"/>
+      <c r="B295">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C295">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D292">
-        <f t="shared" si="30"/>
+      <c r="D295">
+        <f t="shared" si="42"/>
         <v>14</v>
       </c>
-      <c r="E292">
-        <f t="shared" si="31"/>
+      <c r="E295">
+        <f t="shared" si="43"/>
         <v>42</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A293" s="1">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A296" s="1">
         <v>43753</v>
       </c>
-      <c r="B293">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C293">
-        <f t="shared" si="29"/>
+      <c r="B296">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C296">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D293">
-        <f t="shared" si="30"/>
+      <c r="D296">
+        <f t="shared" si="42"/>
         <v>15</v>
       </c>
-      <c r="E293">
-        <f t="shared" si="31"/>
+      <c r="E296">
+        <f t="shared" si="43"/>
         <v>42</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A294" s="1">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A297" s="1">
         <v>43754</v>
       </c>
-      <c r="B294">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C294">
-        <f t="shared" si="29"/>
+      <c r="B297">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C297">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D294">
-        <f t="shared" si="30"/>
+      <c r="D297">
+        <f t="shared" si="42"/>
         <v>16</v>
       </c>
-      <c r="E294">
-        <f t="shared" si="31"/>
+      <c r="E297">
+        <f t="shared" si="43"/>
         <v>42</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A295" s="1">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A298" s="1">
         <v>43755</v>
       </c>
-      <c r="B295">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C295">
-        <f t="shared" si="29"/>
+      <c r="B298">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C298">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D295">
-        <f t="shared" si="30"/>
+      <c r="D298">
+        <f t="shared" si="42"/>
         <v>17</v>
       </c>
-      <c r="E295">
-        <f t="shared" si="31"/>
+      <c r="E298">
+        <f t="shared" si="43"/>
         <v>42</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A296" s="1">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A299" s="1">
         <v>43756</v>
       </c>
-      <c r="B296">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C296">
-        <f t="shared" si="29"/>
+      <c r="B299">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C299">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D296">
-        <f t="shared" si="30"/>
+      <c r="D299">
+        <f t="shared" si="42"/>
         <v>18</v>
       </c>
-      <c r="E296">
-        <f t="shared" si="31"/>
+      <c r="E299">
+        <f t="shared" si="43"/>
         <v>42</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A297" s="1">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A300" s="1">
         <v>43757</v>
       </c>
-      <c r="B297">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C297">
-        <f t="shared" si="29"/>
+      <c r="B300">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C300">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D297">
-        <f t="shared" si="30"/>
+      <c r="D300">
+        <f t="shared" si="42"/>
         <v>19</v>
       </c>
-      <c r="E297">
-        <f t="shared" si="31"/>
+      <c r="E300">
+        <f t="shared" si="43"/>
         <v>42</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A298" s="1">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A301" s="1">
         <v>43758</v>
       </c>
-      <c r="B298">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C298">
-        <f t="shared" si="29"/>
+      <c r="B301">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C301">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D298">
-        <f t="shared" si="30"/>
+      <c r="D301">
+        <f t="shared" si="42"/>
         <v>20</v>
       </c>
-      <c r="E298">
-        <f t="shared" si="31"/>
+      <c r="E301">
+        <f t="shared" si="43"/>
         <v>43</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A299" s="1">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A302" s="1">
         <v>43759</v>
       </c>
-      <c r="B299">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C299">
-        <f t="shared" si="29"/>
+      <c r="B302">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C302">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D299">
-        <f t="shared" si="30"/>
+      <c r="D302">
+        <f t="shared" si="42"/>
         <v>21</v>
       </c>
-      <c r="E299">
-        <f t="shared" si="31"/>
+      <c r="E302">
+        <f t="shared" si="43"/>
         <v>43</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A300" s="1">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A303" s="1">
         <v>43760</v>
       </c>
-      <c r="B300">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C300">
-        <f t="shared" si="29"/>
+      <c r="B303">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C303">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D300">
-        <f t="shared" si="30"/>
+      <c r="D303">
+        <f t="shared" si="42"/>
         <v>22</v>
       </c>
-      <c r="E300">
-        <f t="shared" si="31"/>
+      <c r="E303">
+        <f t="shared" si="43"/>
         <v>43</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A301" s="1">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A304" s="1">
         <v>43761</v>
       </c>
-      <c r="B301">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C301">
-        <f t="shared" si="29"/>
+      <c r="B304">
+        <f t="shared" si="40"/>
+        <v>2019</v>
+      </c>
+      <c r="C304">
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
-      <c r="D301">
-        <f t="shared" si="30"/>
+      <c r="D304">
+        <f t="shared" si="42"/>
         <v>23</v>
       </c>
-      <c r="E301">
-        <f t="shared" si="31"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A302" s="1">
-        <v>43762</v>
-      </c>
-      <c r="B302">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C302">
-        <f t="shared" si="29"/>
-        <v>10</v>
-      </c>
-      <c r="D302">
-        <f t="shared" si="30"/>
-        <v>24</v>
-      </c>
-      <c r="E302">
-        <f t="shared" si="31"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A303" s="1">
-        <v>43763</v>
-      </c>
-      <c r="B303">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C303">
-        <f t="shared" si="29"/>
-        <v>10</v>
-      </c>
-      <c r="D303">
-        <f t="shared" si="30"/>
-        <v>25</v>
-      </c>
-      <c r="E303">
-        <f t="shared" si="31"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A304" s="1">
-        <v>43764</v>
-      </c>
-      <c r="B304">
-        <f t="shared" si="28"/>
-        <v>2019</v>
-      </c>
-      <c r="C304">
-        <f t="shared" si="29"/>
-        <v>10</v>
-      </c>
-      <c r="D304">
-        <f t="shared" si="30"/>
-        <v>26</v>
-      </c>
       <c r="E304">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>43</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
-        <v>43765</v>
+        <v>43762</v>
       </c>
       <c r="B305">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C305">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
       <c r="D305">
-        <f t="shared" si="30"/>
-        <v>27</v>
+        <f t="shared" si="42"/>
+        <v>24</v>
       </c>
       <c r="E305">
-        <f t="shared" si="31"/>
-        <v>44</v>
+        <f t="shared" si="43"/>
+        <v>43</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
-        <v>43766</v>
+        <v>43763</v>
       </c>
       <c r="B306">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C306">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
       <c r="D306">
-        <f t="shared" si="30"/>
-        <v>28</v>
+        <f t="shared" si="42"/>
+        <v>25</v>
       </c>
       <c r="E306">
-        <f t="shared" si="31"/>
-        <v>44</v>
+        <f t="shared" si="43"/>
+        <v>43</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
-        <v>43767</v>
+        <v>43764</v>
       </c>
       <c r="B307">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C307">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
       <c r="D307">
-        <f t="shared" si="30"/>
-        <v>29</v>
+        <f t="shared" si="42"/>
+        <v>26</v>
       </c>
       <c r="E307">
-        <f t="shared" si="31"/>
-        <v>44</v>
+        <f t="shared" si="43"/>
+        <v>43</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
-        <v>43768</v>
+        <v>43765</v>
       </c>
       <c r="B308">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C308">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
       <c r="D308">
-        <f t="shared" si="30"/>
-        <v>30</v>
+        <f t="shared" si="42"/>
+        <v>27</v>
       </c>
       <c r="E308">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>44</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
-        <v>43769</v>
+        <v>43766</v>
       </c>
       <c r="B309">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C309">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
       <c r="D309">
-        <f t="shared" si="30"/>
-        <v>31</v>
+        <f t="shared" si="42"/>
+        <v>28</v>
       </c>
       <c r="E309">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>44</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
-        <v>43770</v>
+        <v>43767</v>
       </c>
       <c r="B310">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C310">
-        <f t="shared" si="29"/>
-        <v>11</v>
+        <f t="shared" si="41"/>
+        <v>10</v>
       </c>
       <c r="D310">
-        <f t="shared" si="30"/>
-        <v>1</v>
+        <f t="shared" si="42"/>
+        <v>29</v>
       </c>
       <c r="E310">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>44</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
-        <v>43771</v>
+        <v>43768</v>
       </c>
       <c r="B311">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C311">
-        <f t="shared" si="29"/>
-        <v>11</v>
+        <f t="shared" si="41"/>
+        <v>10</v>
       </c>
       <c r="D311">
-        <f t="shared" si="30"/>
-        <v>2</v>
+        <f t="shared" si="42"/>
+        <v>30</v>
       </c>
       <c r="E311">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>44</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
-        <v>43772</v>
+        <v>43769</v>
       </c>
       <c r="B312">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C312">
-        <f t="shared" si="29"/>
-        <v>11</v>
+        <f t="shared" si="41"/>
+        <v>10</v>
       </c>
       <c r="D312">
-        <f t="shared" si="30"/>
-        <v>3</v>
+        <f t="shared" si="42"/>
+        <v>31</v>
       </c>
       <c r="E312">
-        <f t="shared" si="31"/>
-        <v>45</v>
+        <f t="shared" si="43"/>
+        <v>44</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
-        <v>43773</v>
+        <v>43770</v>
       </c>
       <c r="B313">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C313">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D313">
-        <f t="shared" si="30"/>
-        <v>4</v>
+        <f t="shared" si="42"/>
+        <v>1</v>
       </c>
       <c r="E313">
-        <f t="shared" si="31"/>
-        <v>45</v>
+        <f t="shared" si="43"/>
+        <v>44</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
-        <v>43774</v>
+        <v>43771</v>
       </c>
       <c r="B314">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C314">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D314">
-        <f t="shared" si="30"/>
-        <v>5</v>
+        <f t="shared" si="42"/>
+        <v>2</v>
       </c>
       <c r="E314">
-        <f t="shared" si="31"/>
-        <v>45</v>
+        <f t="shared" si="43"/>
+        <v>44</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
-        <v>43775</v>
+        <v>43772</v>
       </c>
       <c r="B315">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C315">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D315">
-        <f t="shared" si="30"/>
-        <v>6</v>
+        <f t="shared" si="42"/>
+        <v>3</v>
       </c>
       <c r="E315">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>45</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
-        <v>43776</v>
+        <v>43773</v>
       </c>
       <c r="B316">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C316">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D316">
-        <f t="shared" si="30"/>
-        <v>7</v>
+        <f t="shared" si="42"/>
+        <v>4</v>
       </c>
       <c r="E316">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>45</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
-        <v>43777</v>
+        <v>43774</v>
       </c>
       <c r="B317">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C317">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D317">
-        <f t="shared" si="30"/>
-        <v>8</v>
+        <f t="shared" si="42"/>
+        <v>5</v>
       </c>
       <c r="E317">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>45</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
-        <v>43778</v>
+        <v>43775</v>
       </c>
       <c r="B318">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C318">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D318">
-        <f t="shared" si="30"/>
-        <v>9</v>
+        <f t="shared" si="42"/>
+        <v>6</v>
       </c>
       <c r="E318">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>45</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
-        <v>43779</v>
+        <v>43776</v>
       </c>
       <c r="B319">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C319">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D319">
-        <f t="shared" si="30"/>
-        <v>10</v>
+        <f t="shared" si="42"/>
+        <v>7</v>
       </c>
       <c r="E319">
-        <f t="shared" si="31"/>
-        <v>46</v>
+        <f t="shared" si="43"/>
+        <v>45</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
-        <v>43780</v>
+        <v>43777</v>
       </c>
       <c r="B320">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C320">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D320">
-        <f t="shared" si="30"/>
-        <v>11</v>
+        <f t="shared" si="42"/>
+        <v>8</v>
       </c>
       <c r="E320">
-        <f t="shared" si="31"/>
-        <v>46</v>
+        <f t="shared" si="43"/>
+        <v>45</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
-        <v>43781</v>
+        <v>43778</v>
       </c>
       <c r="B321">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C321">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D321">
-        <f t="shared" si="30"/>
-        <v>12</v>
+        <f t="shared" si="42"/>
+        <v>9</v>
       </c>
       <c r="E321">
-        <f t="shared" si="31"/>
-        <v>46</v>
+        <f t="shared" si="43"/>
+        <v>45</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
-        <v>43782</v>
+        <v>43779</v>
       </c>
       <c r="B322">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C322">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D322">
-        <f t="shared" si="30"/>
-        <v>13</v>
+        <f t="shared" si="42"/>
+        <v>10</v>
       </c>
       <c r="E322">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>46</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
-        <v>43783</v>
+        <v>43780</v>
       </c>
       <c r="B323">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C323">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D323">
-        <f t="shared" si="30"/>
-        <v>14</v>
+        <f t="shared" si="42"/>
+        <v>11</v>
       </c>
       <c r="E323">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>46</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
-        <v>43784</v>
+        <v>43781</v>
       </c>
       <c r="B324">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C324">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D324">
-        <f t="shared" si="30"/>
-        <v>15</v>
+        <f t="shared" si="42"/>
+        <v>12</v>
       </c>
       <c r="E324">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>46</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
-        <v>43785</v>
+        <v>43782</v>
       </c>
       <c r="B325">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C325">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D325">
-        <f t="shared" si="30"/>
-        <v>16</v>
+        <f t="shared" si="42"/>
+        <v>13</v>
       </c>
       <c r="E325">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>46</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
-        <v>43786</v>
+        <v>43783</v>
       </c>
       <c r="B326">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C326">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D326">
-        <f t="shared" si="30"/>
-        <v>17</v>
+        <f t="shared" si="42"/>
+        <v>14</v>
       </c>
       <c r="E326">
-        <f t="shared" si="31"/>
-        <v>47</v>
+        <f t="shared" si="43"/>
+        <v>46</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
-        <v>43787</v>
+        <v>43784</v>
       </c>
       <c r="B327">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C327">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D327">
-        <f t="shared" si="30"/>
-        <v>18</v>
+        <f t="shared" si="42"/>
+        <v>15</v>
       </c>
       <c r="E327">
-        <f t="shared" si="31"/>
-        <v>47</v>
+        <f t="shared" si="43"/>
+        <v>46</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
-        <v>43788</v>
+        <v>43785</v>
       </c>
       <c r="B328">
-        <f t="shared" si="28"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C328">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D328">
-        <f t="shared" si="30"/>
-        <v>19</v>
+        <f t="shared" si="42"/>
+        <v>16</v>
       </c>
       <c r="E328">
-        <f t="shared" si="31"/>
-        <v>47</v>
+        <f t="shared" si="43"/>
+        <v>46</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
-        <v>43789</v>
+        <v>43786</v>
       </c>
       <c r="B329">
-        <f t="shared" ref="B329:B370" si="32">YEAR(A329)</f>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C329">
-        <f t="shared" ref="C329:C370" si="33">MONTH(A329)</f>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D329">
-        <f t="shared" ref="D329:D370" si="34">DAY(A329)</f>
-        <v>20</v>
+        <f t="shared" si="42"/>
+        <v>17</v>
       </c>
       <c r="E329">
-        <f t="shared" ref="E329:E370" si="35">WEEKNUM(A329)</f>
+        <f t="shared" si="43"/>
         <v>47</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
-        <v>43790</v>
+        <v>43787</v>
       </c>
       <c r="B330">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C330">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D330">
-        <f t="shared" si="34"/>
-        <v>21</v>
+        <f t="shared" si="42"/>
+        <v>18</v>
       </c>
       <c r="E330">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>47</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
-        <v>43791</v>
+        <v>43788</v>
       </c>
       <c r="B331">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>2019</v>
       </c>
       <c r="C331">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D331">
-        <f t="shared" si="34"/>
-        <v>22</v>
+        <f t="shared" si="42"/>
+        <v>19</v>
       </c>
       <c r="E331">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>47</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
-        <v>43792</v>
+        <v>43789</v>
       </c>
       <c r="B332">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="B332:B373" si="44">YEAR(A332)</f>
         <v>2019</v>
       </c>
       <c r="C332">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="C332:C373" si="45">MONTH(A332)</f>
         <v>11</v>
       </c>
       <c r="D332">
-        <f t="shared" si="34"/>
-        <v>23</v>
+        <f t="shared" ref="D332:D373" si="46">DAY(A332)</f>
+        <v>20</v>
       </c>
       <c r="E332">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="E332:E373" si="47">WEEKNUM(A332)</f>
         <v>47</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
-        <v>43793</v>
+        <v>43790</v>
       </c>
       <c r="B333">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C333">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>11</v>
       </c>
       <c r="D333">
-        <f t="shared" si="34"/>
-        <v>24</v>
+        <f t="shared" si="46"/>
+        <v>21</v>
       </c>
       <c r="E333">
-        <f t="shared" si="35"/>
-        <v>48</v>
+        <f t="shared" si="47"/>
+        <v>47</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
-        <v>43794</v>
+        <v>43791</v>
       </c>
       <c r="B334">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C334">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>11</v>
       </c>
       <c r="D334">
-        <f t="shared" si="34"/>
-        <v>25</v>
+        <f t="shared" si="46"/>
+        <v>22</v>
       </c>
       <c r="E334">
-        <f t="shared" si="35"/>
-        <v>48</v>
+        <f t="shared" si="47"/>
+        <v>47</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
-        <v>43795</v>
+        <v>43792</v>
       </c>
       <c r="B335">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C335">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>11</v>
       </c>
       <c r="D335">
-        <f t="shared" si="34"/>
-        <v>26</v>
+        <f t="shared" si="46"/>
+        <v>23</v>
       </c>
       <c r="E335">
-        <f t="shared" si="35"/>
-        <v>48</v>
+        <f t="shared" si="47"/>
+        <v>47</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
-        <v>43796</v>
+        <v>43793</v>
       </c>
       <c r="B336">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C336">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>11</v>
       </c>
       <c r="D336">
-        <f t="shared" si="34"/>
-        <v>27</v>
+        <f t="shared" si="46"/>
+        <v>24</v>
       </c>
       <c r="E336">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>48</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
-        <v>43797</v>
+        <v>43794</v>
       </c>
       <c r="B337">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C337">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>11</v>
       </c>
       <c r="D337">
-        <f t="shared" si="34"/>
-        <v>28</v>
+        <f t="shared" si="46"/>
+        <v>25</v>
       </c>
       <c r="E337">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>48</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
-        <v>43798</v>
+        <v>43795</v>
       </c>
       <c r="B338">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C338">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>11</v>
       </c>
       <c r="D338">
-        <f t="shared" si="34"/>
-        <v>29</v>
+        <f t="shared" si="46"/>
+        <v>26</v>
       </c>
       <c r="E338">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>48</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
-        <v>43799</v>
+        <v>43796</v>
       </c>
       <c r="B339">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C339">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>11</v>
       </c>
       <c r="D339">
-        <f t="shared" si="34"/>
-        <v>30</v>
+        <f t="shared" si="46"/>
+        <v>27</v>
       </c>
       <c r="E339">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>48</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
-        <v>43800</v>
+        <v>43797</v>
       </c>
       <c r="B340">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C340">
-        <f t="shared" si="33"/>
-        <v>12</v>
+        <f t="shared" si="45"/>
+        <v>11</v>
       </c>
       <c r="D340">
-        <f t="shared" si="34"/>
-        <v>1</v>
+        <f t="shared" si="46"/>
+        <v>28</v>
       </c>
       <c r="E340">
-        <f t="shared" si="35"/>
-        <v>49</v>
+        <f t="shared" si="47"/>
+        <v>48</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
-        <v>43801</v>
+        <v>43798</v>
       </c>
       <c r="B341">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C341">
-        <f t="shared" si="33"/>
-        <v>12</v>
+        <f t="shared" si="45"/>
+        <v>11</v>
       </c>
       <c r="D341">
-        <f t="shared" si="34"/>
-        <v>2</v>
+        <f t="shared" si="46"/>
+        <v>29</v>
       </c>
       <c r="E341">
-        <f t="shared" si="35"/>
-        <v>49</v>
+        <f t="shared" si="47"/>
+        <v>48</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
-        <v>43802</v>
+        <v>43799</v>
       </c>
       <c r="B342">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C342">
-        <f t="shared" si="33"/>
-        <v>12</v>
+        <f t="shared" si="45"/>
+        <v>11</v>
       </c>
       <c r="D342">
-        <f t="shared" si="34"/>
-        <v>3</v>
+        <f t="shared" si="46"/>
+        <v>30</v>
       </c>
       <c r="E342">
-        <f t="shared" si="35"/>
-        <v>49</v>
+        <f t="shared" si="47"/>
+        <v>48</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A343" s="1">
-        <v>43803</v>
+        <v>43800</v>
       </c>
       <c r="B343">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C343">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D343">
-        <f t="shared" si="34"/>
-        <v>4</v>
+        <f t="shared" si="46"/>
+        <v>1</v>
       </c>
       <c r="E343">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>49</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A344" s="1">
-        <v>43804</v>
+        <v>43801</v>
       </c>
       <c r="B344">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C344">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D344">
-        <f t="shared" si="34"/>
-        <v>5</v>
+        <f t="shared" si="46"/>
+        <v>2</v>
       </c>
       <c r="E344">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>49</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A345" s="1">
-        <v>43805</v>
+        <v>43802</v>
       </c>
       <c r="B345">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C345">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D345">
-        <f t="shared" si="34"/>
-        <v>6</v>
+        <f t="shared" si="46"/>
+        <v>3</v>
       </c>
       <c r="E345">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>49</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A346" s="1">
-        <v>43806</v>
+        <v>43803</v>
       </c>
       <c r="B346">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C346">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D346">
-        <f t="shared" si="34"/>
-        <v>7</v>
+        <f t="shared" si="46"/>
+        <v>4</v>
       </c>
       <c r="E346">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>49</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A347" s="1">
-        <v>43807</v>
+        <v>43804</v>
       </c>
       <c r="B347">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C347">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D347">
-        <f t="shared" si="34"/>
-        <v>8</v>
+        <f t="shared" si="46"/>
+        <v>5</v>
       </c>
       <c r="E347">
-        <f t="shared" si="35"/>
-        <v>50</v>
+        <f t="shared" si="47"/>
+        <v>49</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A348" s="1">
-        <v>43808</v>
+        <v>43805</v>
       </c>
       <c r="B348">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C348">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D348">
-        <f t="shared" si="34"/>
-        <v>9</v>
+        <f t="shared" si="46"/>
+        <v>6</v>
       </c>
       <c r="E348">
-        <f t="shared" si="35"/>
-        <v>50</v>
+        <f t="shared" si="47"/>
+        <v>49</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
-        <v>43809</v>
+        <v>43806</v>
       </c>
       <c r="B349">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C349">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D349">
-        <f t="shared" si="34"/>
-        <v>10</v>
+        <f t="shared" si="46"/>
+        <v>7</v>
       </c>
       <c r="E349">
-        <f t="shared" si="35"/>
-        <v>50</v>
+        <f t="shared" si="47"/>
+        <v>49</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
-        <v>43810</v>
+        <v>43807</v>
       </c>
       <c r="B350">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C350">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D350">
-        <f t="shared" si="34"/>
-        <v>11</v>
+        <f t="shared" si="46"/>
+        <v>8</v>
       </c>
       <c r="E350">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>50</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
-        <v>43811</v>
+        <v>43808</v>
       </c>
       <c r="B351">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C351">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D351">
-        <f t="shared" si="34"/>
-        <v>12</v>
+        <f t="shared" si="46"/>
+        <v>9</v>
       </c>
       <c r="E351">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>50</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
-        <v>43812</v>
+        <v>43809</v>
       </c>
       <c r="B352">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C352">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D352">
-        <f t="shared" si="34"/>
-        <v>13</v>
+        <f t="shared" si="46"/>
+        <v>10</v>
       </c>
       <c r="E352">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>50</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
-        <v>43813</v>
+        <v>43810</v>
       </c>
       <c r="B353">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C353">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D353">
-        <f t="shared" si="34"/>
-        <v>14</v>
+        <f t="shared" si="46"/>
+        <v>11</v>
       </c>
       <c r="E353">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>50</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
-        <v>43814</v>
+        <v>43811</v>
       </c>
       <c r="B354">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C354">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D354">
-        <f t="shared" si="34"/>
-        <v>15</v>
+        <f t="shared" si="46"/>
+        <v>12</v>
       </c>
       <c r="E354">
-        <f t="shared" si="35"/>
-        <v>51</v>
+        <f t="shared" si="47"/>
+        <v>50</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
-        <v>43815</v>
+        <v>43812</v>
       </c>
       <c r="B355">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C355">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D355">
-        <f t="shared" si="34"/>
-        <v>16</v>
+        <f t="shared" si="46"/>
+        <v>13</v>
       </c>
       <c r="E355">
-        <f t="shared" si="35"/>
-        <v>51</v>
+        <f t="shared" si="47"/>
+        <v>50</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
-        <v>43816</v>
+        <v>43813</v>
       </c>
       <c r="B356">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C356">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D356">
-        <f t="shared" si="34"/>
-        <v>17</v>
+        <f t="shared" si="46"/>
+        <v>14</v>
       </c>
       <c r="E356">
-        <f t="shared" si="35"/>
-        <v>51</v>
+        <f t="shared" si="47"/>
+        <v>50</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
-        <v>43817</v>
+        <v>43814</v>
       </c>
       <c r="B357">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C357">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D357">
-        <f t="shared" si="34"/>
-        <v>18</v>
+        <f t="shared" si="46"/>
+        <v>15</v>
       </c>
       <c r="E357">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>51</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
-        <v>43818</v>
+        <v>43815</v>
       </c>
       <c r="B358">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C358">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D358">
-        <f t="shared" si="34"/>
-        <v>19</v>
+        <f t="shared" si="46"/>
+        <v>16</v>
       </c>
       <c r="E358">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>51</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A359" s="1">
-        <v>43819</v>
+        <v>43816</v>
       </c>
       <c r="B359">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C359">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D359">
-        <f t="shared" si="34"/>
-        <v>20</v>
+        <f t="shared" si="46"/>
+        <v>17</v>
       </c>
       <c r="E359">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>51</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A360" s="1">
-        <v>43820</v>
+        <v>43817</v>
       </c>
       <c r="B360">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C360">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D360">
-        <f t="shared" si="34"/>
-        <v>21</v>
+        <f t="shared" si="46"/>
+        <v>18</v>
       </c>
       <c r="E360">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>51</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
-        <v>43821</v>
+        <v>43818</v>
       </c>
       <c r="B361">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C361">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D361">
-        <f t="shared" si="34"/>
-        <v>22</v>
+        <f t="shared" si="46"/>
+        <v>19</v>
       </c>
       <c r="E361">
-        <f t="shared" si="35"/>
-        <v>52</v>
+        <f t="shared" si="47"/>
+        <v>51</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
-        <v>43822</v>
+        <v>43819</v>
       </c>
       <c r="B362">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C362">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D362">
-        <f t="shared" si="34"/>
-        <v>23</v>
+        <f t="shared" si="46"/>
+        <v>20</v>
       </c>
       <c r="E362">
-        <f t="shared" si="35"/>
-        <v>52</v>
+        <f t="shared" si="47"/>
+        <v>51</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A363" s="1">
-        <v>43823</v>
+        <v>43820</v>
       </c>
       <c r="B363">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C363">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D363">
-        <f t="shared" si="34"/>
-        <v>24</v>
+        <f t="shared" si="46"/>
+        <v>21</v>
       </c>
       <c r="E363">
-        <f t="shared" si="35"/>
-        <v>52</v>
+        <f t="shared" si="47"/>
+        <v>51</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A364" s="1">
-        <v>43824</v>
+        <v>43821</v>
       </c>
       <c r="B364">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C364">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D364">
-        <f t="shared" si="34"/>
-        <v>25</v>
+        <f t="shared" si="46"/>
+        <v>22</v>
       </c>
       <c r="E364">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>52</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
-        <v>43825</v>
+        <v>43822</v>
       </c>
       <c r="B365">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C365">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D365">
-        <f t="shared" si="34"/>
-        <v>26</v>
+        <f t="shared" si="46"/>
+        <v>23</v>
       </c>
       <c r="E365">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>52</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A366" s="1">
-        <v>43826</v>
+        <v>43823</v>
       </c>
       <c r="B366">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C366">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D366">
-        <f t="shared" si="34"/>
-        <v>27</v>
+        <f t="shared" si="46"/>
+        <v>24</v>
       </c>
       <c r="E366">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>52</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A367" s="1">
-        <v>43827</v>
+        <v>43824</v>
       </c>
       <c r="B367">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C367">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D367">
-        <f t="shared" si="34"/>
-        <v>28</v>
+        <f t="shared" si="46"/>
+        <v>25</v>
       </c>
       <c r="E367">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>52</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A368" s="1">
-        <v>43828</v>
+        <v>43825</v>
       </c>
       <c r="B368">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C368">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D368">
-        <f t="shared" si="34"/>
-        <v>29</v>
+        <f t="shared" si="46"/>
+        <v>26</v>
       </c>
       <c r="E368">
-        <f t="shared" si="35"/>
-        <v>53</v>
+        <f t="shared" si="47"/>
+        <v>52</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A369" s="1">
-        <v>43829</v>
+        <v>43826</v>
       </c>
       <c r="B369">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>2019</v>
       </c>
       <c r="C369">
-        <f t="shared" si="33"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="D369">
-        <f t="shared" si="34"/>
-        <v>30</v>
+        <f t="shared" si="46"/>
+        <v>27</v>
       </c>
       <c r="E369">
-        <f t="shared" si="35"/>
-        <v>53</v>
+        <f t="shared" si="47"/>
+        <v>52</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A370" s="1">
+        <v>43827</v>
+      </c>
+      <c r="B370">
+        <f t="shared" si="44"/>
+        <v>2019</v>
+      </c>
+      <c r="C370">
+        <f t="shared" si="45"/>
+        <v>12</v>
+      </c>
+      <c r="D370">
+        <f t="shared" si="46"/>
+        <v>28</v>
+      </c>
+      <c r="E370">
+        <f t="shared" si="47"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="371" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A371" s="1">
+        <v>43828</v>
+      </c>
+      <c r="B371">
+        <f t="shared" si="44"/>
+        <v>2019</v>
+      </c>
+      <c r="C371">
+        <f t="shared" si="45"/>
+        <v>12</v>
+      </c>
+      <c r="D371">
+        <f t="shared" si="46"/>
+        <v>29</v>
+      </c>
+      <c r="E371">
+        <f t="shared" si="47"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="372" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A372" s="1">
+        <v>43829</v>
+      </c>
+      <c r="B372">
+        <f t="shared" si="44"/>
+        <v>2019</v>
+      </c>
+      <c r="C372">
+        <f t="shared" si="45"/>
+        <v>12</v>
+      </c>
+      <c r="D372">
+        <f t="shared" si="46"/>
+        <v>30</v>
+      </c>
+      <c r="E372">
+        <f t="shared" si="47"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="373" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A373" s="1">
         <v>43830</v>
       </c>
-      <c r="B370">
-        <f t="shared" si="32"/>
-        <v>2019</v>
-      </c>
-      <c r="C370">
-        <f t="shared" si="33"/>
+      <c r="B373">
+        <f t="shared" si="44"/>
+        <v>2019</v>
+      </c>
+      <c r="C373">
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
-      <c r="D370">
-        <f t="shared" si="34"/>
+      <c r="D373">
+        <f t="shared" si="46"/>
         <v>31</v>
       </c>
-      <c r="E370">
-        <f t="shared" si="35"/>
+      <c r="E373">
+        <f t="shared" si="47"/>
         <v>53</v>
       </c>
     </row>
@@ -9641,10 +10059,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082B48B6-1501-774C-818C-F75B39B01AEE}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9794,6 +10212,20 @@
         <v>27</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>2018</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>